<commit_message>
#2 update mock up file compare
</commit_message>
<xml_diff>
--- a/test/Cactus.MiniExcelConverterTest/Features/SampleTest.xlsx
+++ b/test/Cactus.MiniExcelConverterTest/Features/SampleTest.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.MiniExcelConverterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38107619-39CC-474D-ADBA-26679F359453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8834315-4E0C-4B41-89FE-A90C3317E3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SampleTest" sheetId="1" r:id="rId1"/>
+    <sheet name="SampleTest1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateCount="250" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -386,7 +386,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>